<commit_message>
Reorganization of repository and version 0 of methods and preliminary results
</commit_message>
<xml_diff>
--- a/results/supplementary/FAME's list.xlsx
+++ b/results/supplementary/FAME's list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/ageing/results/supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9C14B3F-4E9F-4FC0-98DA-759346E6EBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F9C14B3F-4E9F-4FC0-98DA-759346E6EBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE417B41-D9D3-49C9-9A52-EA253B56D585}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B88F95DF-C4FE-4A7C-987E-5FCB7A36026A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B88F95DF-C4FE-4A7C-987E-5FCB7A36026A}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLA COMPUESTOS" sheetId="1" r:id="rId1"/>
@@ -914,25 +914,7 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -942,9 +924,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -988,8 +967,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,7 +1330,7 @@
   </sheetPr>
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1341,510 +1341,510 @@
     <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="24"/>
+      <c r="C29" s="17"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="15" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="22"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="22"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="15" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="15" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="22"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="15" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="22"/>
+      <c r="C42" s="15"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="15" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="22"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="15" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="21" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Complementary results to supplementary
</commit_message>
<xml_diff>
--- a/results/supplementary/FAME's list.xlsx
+++ b/results/supplementary/FAME's list.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - Universidad de Oviedo\IMIB\Softwares\GitHub\Oilcontent_Longevity\results\supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F9C14B3F-4E9F-4FC0-98DA-759346E6EBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE417B41-D9D3-49C9-9A52-EA253B56D585}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B88F95DF-C4FE-4A7C-987E-5FCB7A36026A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="TABLA COMPUESTOS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>TABLAS DE COMPUESTOS POSIBLES DE IDENTIFICAR</t>
   </si>
@@ -631,9 +630,6 @@
     </r>
   </si>
   <si>
-    <t>La Unidad realiza el análisis de los ésteres metílicos de los ácidos grasos que aparecen en la siguiente tabla</t>
-  </si>
-  <si>
     <t>Abreviation</t>
   </si>
   <si>
@@ -646,8 +642,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -912,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -967,6 +963,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -984,12 +983,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,60 +1317,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297F1222-56C3-46A4-B9DA-ECED8CBA59AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1">
       <c r="A3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -1388,7 +1381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1399,7 +1392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1410,7 +1403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1421,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1432,7 +1425,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -1443,7 +1436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -1454,7 +1447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1465,7 +1458,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15">
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
@@ -1476,7 +1469,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -1485,7 +1478,7 @@
       </c>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -1496,7 +1489,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
@@ -1507,7 +1500,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
@@ -1516,7 +1509,7 @@
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -1525,7 +1518,7 @@
       </c>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1536,7 +1529,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" s="7" t="s">
         <v>47</v>
       </c>
@@ -1545,7 +1538,7 @@
       </c>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="7" t="s">
         <v>49</v>
       </c>
@@ -1556,7 +1549,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -1567,7 +1560,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="7" t="s">
         <v>55</v>
       </c>
@@ -1578,7 +1571,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15">
       <c r="A24" s="7" t="s">
         <v>58</v>
       </c>
@@ -1589,7 +1582,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15">
       <c r="A25" s="13" t="s">
         <v>61</v>
       </c>
@@ -1600,7 +1593,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="13" t="s">
         <v>64</v>
       </c>
@@ -1611,7 +1604,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15">
       <c r="A27" s="13" t="s">
         <v>67</v>
       </c>
@@ -1622,7 +1615,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" s="13" t="s">
         <v>70</v>
       </c>
@@ -1633,7 +1626,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15">
       <c r="A29" s="13" t="s">
         <v>73</v>
       </c>
@@ -1642,7 +1635,7 @@
       </c>
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" s="13" t="s">
         <v>75</v>
       </c>
@@ -1653,7 +1646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15">
       <c r="A31" s="13" t="s">
         <v>78</v>
       </c>
@@ -1664,7 +1657,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15">
       <c r="A32" s="13" t="s">
         <v>81</v>
       </c>
@@ -1673,7 +1666,7 @@
       </c>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" s="13" t="s">
         <v>83</v>
       </c>
@@ -1682,7 +1675,7 @@
       </c>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15">
       <c r="A34" s="13" t="s">
         <v>85</v>
       </c>
@@ -1693,7 +1686,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15">
       <c r="A35" s="13" t="s">
         <v>88</v>
       </c>
@@ -1702,7 +1695,7 @@
       </c>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15">
       <c r="A36" s="13" t="s">
         <v>90</v>
       </c>
@@ -1713,7 +1706,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" s="13" t="s">
         <v>93</v>
       </c>
@@ -1724,7 +1717,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15">
       <c r="A38" s="13" t="s">
         <v>96</v>
       </c>
@@ -1735,7 +1728,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15">
       <c r="A39" s="13" t="s">
         <v>99</v>
       </c>
@@ -1744,7 +1737,7 @@
       </c>
       <c r="C39" s="15"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15">
       <c r="A40" s="13" t="s">
         <v>101</v>
       </c>
@@ -1755,7 +1748,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15">
       <c r="A41" s="13" t="s">
         <v>104</v>
       </c>
@@ -1766,7 +1759,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15">
       <c r="A42" s="13" t="s">
         <v>107</v>
       </c>
@@ -1775,7 +1768,7 @@
       </c>
       <c r="C42" s="15"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15">
       <c r="A43" s="13" t="s">
         <v>109</v>
       </c>
@@ -1786,7 +1779,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15">
       <c r="A44" s="13" t="s">
         <v>112</v>
       </c>
@@ -1797,7 +1790,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15">
       <c r="A45" s="13" t="s">
         <v>115</v>
       </c>
@@ -1808,7 +1801,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15">
       <c r="A46" s="13" t="s">
         <v>118</v>
       </c>
@@ -1817,7 +1810,7 @@
       </c>
       <c r="C46" s="15"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15">
       <c r="A47" s="13" t="s">
         <v>120</v>
       </c>
@@ -1828,7 +1821,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" thickBot="1">
       <c r="A48" s="19" t="s">
         <v>123</v>
       </c>
@@ -1839,18 +1832,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A50:C50"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>

</xml_diff>